<commit_message>
added modified homework 4
</commit_message>
<xml_diff>
--- a/Homework/Lesson4/Scenarios.xlsx
+++ b/Homework/Lesson4/Scenarios.xlsx
@@ -54,9 +54,6 @@
     <t>check available meal included in AirAsia airline</t>
   </si>
   <si>
-    <t>Ecpected result</t>
-  </si>
-  <si>
     <t>Test case</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>1006, 1007, 1008</t>
+  </si>
+  <si>
+    <t>Expected result</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,10 +502,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,10 +513,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,7 +527,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -549,7 +549,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,7 +560,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -571,7 +571,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -582,7 +582,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -615,7 +615,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,10 +641,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -652,10 +652,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,10 +663,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,10 +674,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -686,10 +686,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -698,10 +698,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -719,7 +719,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,10 +732,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>